<commit_message>
CTMS Automation: Iniitial checkin; Setup of Login test with IE browser
</commit_message>
<xml_diff>
--- a/src/test/resources/data/DESKTOP_WEB/Login/LoginTestData.xlsx
+++ b/src/test/resources/data/DESKTOP_WEB/Login/LoginTestData.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\CustomFramework\folder\src\test\resources\data\DESKTOP_WEB\Login\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF7AF80-9361-4B4E-BFDC-D4981F49C7ED}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,55 +19,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Password</t>
-  </si>
-  <si>
-    <t>UserEmail</t>
   </si>
   <si>
     <t>Login_ValidateLoginAndLogout</t>
   </si>
   <si>
-    <t>Login_ValidateErrorMsgForInvalidCredential</t>
+    <t>usersetup</t>
   </si>
   <si>
-    <t>Login_ValidateForgotPassword</t>
+    <t>b1f0rcE</t>
   </si>
   <si>
-    <t>DialogTitle</t>
-  </si>
-  <si>
-    <t>FORGOT YOUR PASSWORD?</t>
-  </si>
-  <si>
-    <t>EmailID</t>
-  </si>
-  <si>
-    <t>atest123010@test.com</t>
-  </si>
-  <si>
-    <t>Username or Password cannot be blank!</t>
-  </si>
-  <si>
-    <t>ErrorMessage</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Login@1234</t>
-  </si>
-  <si>
-    <t>test1@automation.com</t>
+    <t>User</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,7 +151,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -219,7 +186,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -396,93 +363,57 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="44.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="44.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
+    <row r="4" spans="1:4">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
+    <row r="7" spans="1:4">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>